<commit_message>
Update default, fix spelling mistake in Stonington.
</commit_message>
<xml_diff>
--- a/raw/Grand List Data revised 4-2017.xlsx
+++ b/raw/Grand List Data revised 4-2017.xlsx
@@ -6188,7 +6188,7 @@
     <t xml:space="preserve">LTD Properties LLC</t>
   </si>
   <si>
-    <t xml:space="preserve">LSC-Weminster Partnership</t>
+    <t xml:space="preserve">LSC-Westminster Partnership</t>
   </si>
   <si>
     <t xml:space="preserve">Aquarion Water</t>
@@ -6492,17 +6492,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="M/D/YYYY"/>
-    <numFmt numFmtId="169" formatCode="M/D/YYYY"/>
-    <numFmt numFmtId="170" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="MM/DD/YY"/>
+    <numFmt numFmtId="169" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="MM/DD/YY"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -6551,19 +6550,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -6626,13 +6612,13 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6701,43 +6687,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6749,7 +6719,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6801,15 +6771,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6819,14 +6785,6 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -6849,7 +6807,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6872,41 +6830,42 @@
   </sheetPr>
   <dimension ref="A1:AC196"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A151" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D182" activeCellId="0" sqref="D182"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A112" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E138" activeCellId="0" sqref="E138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.8775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.9234693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="257" min="30" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.25"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="257" min="30" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10803,7 +10762,7 @@
         <v>42208</v>
       </c>
     </row>
-    <row r="46" s="26" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" s="22" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="17" t="n">
         <v>1</v>
       </c>
@@ -10811,83 +10770,83 @@
       <c r="C46" s="17" t="s">
         <v>468</v>
       </c>
-      <c r="D46" s="19" t="n">
+      <c r="D46" s="3" t="n">
         <v>2016</v>
       </c>
-      <c r="E46" s="20" t="s">
+      <c r="E46" s="19" t="s">
         <v>469</v>
       </c>
-      <c r="F46" s="21" t="n">
+      <c r="F46" s="5" t="n">
         <v>23790010</v>
       </c>
-      <c r="G46" s="20" t="s">
+      <c r="G46" s="19" t="s">
         <v>470</v>
       </c>
-      <c r="H46" s="21" t="n">
+      <c r="H46" s="5" t="n">
         <v>21834220</v>
       </c>
-      <c r="I46" s="20" t="s">
+      <c r="I46" s="19" t="s">
         <v>471</v>
       </c>
-      <c r="J46" s="21" t="n">
+      <c r="J46" s="5" t="n">
         <v>19261970</v>
       </c>
-      <c r="K46" s="20" t="s">
+      <c r="K46" s="19" t="s">
         <v>472</v>
       </c>
-      <c r="L46" s="22" t="n">
+      <c r="L46" s="20" t="n">
         <v>15501520</v>
       </c>
-      <c r="M46" s="20" t="s">
+      <c r="M46" s="19" t="s">
         <v>473</v>
       </c>
-      <c r="N46" s="21" t="n">
+      <c r="N46" s="5" t="n">
         <v>14993970</v>
       </c>
-      <c r="O46" s="23" t="s">
+      <c r="O46" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="P46" s="21" t="n">
+      <c r="P46" s="5" t="n">
         <v>11063090</v>
       </c>
-      <c r="Q46" s="20" t="s">
+      <c r="Q46" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="R46" s="21" t="n">
+      <c r="R46" s="5" t="n">
         <v>10990100</v>
       </c>
-      <c r="S46" s="20" t="s">
+      <c r="S46" s="19" t="s">
         <v>474</v>
       </c>
-      <c r="T46" s="21" t="n">
+      <c r="T46" s="5" t="n">
         <v>9135090</v>
       </c>
-      <c r="U46" s="20" t="s">
+      <c r="U46" s="19" t="s">
         <v>475</v>
       </c>
-      <c r="V46" s="21" t="n">
+      <c r="V46" s="5" t="n">
         <v>8776440</v>
       </c>
-      <c r="W46" s="20" t="s">
+      <c r="W46" s="19" t="s">
         <v>476</v>
       </c>
-      <c r="X46" s="22" t="n">
+      <c r="X46" s="20" t="n">
         <v>8184460</v>
       </c>
-      <c r="Y46" s="21" t="n">
+      <c r="Y46" s="5" t="n">
         <f aca="false">SUM(E46:X46)</f>
         <v>143530870</v>
       </c>
-      <c r="Z46" s="24" t="n">
+      <c r="Z46" s="6" t="n">
         <v>2016</v>
       </c>
-      <c r="AA46" s="21" t="n">
+      <c r="AA46" s="5" t="n">
         <v>996080360</v>
       </c>
-      <c r="AB46" s="21" t="n">
+      <c r="AB46" s="5" t="n">
         <v>962146920</v>
       </c>
-      <c r="AC46" s="25" t="n">
+      <c r="AC46" s="21" t="n">
         <v>42880</v>
       </c>
     </row>
@@ -11492,7 +11451,7 @@
       <c r="AA53" s="5" t="n">
         <v>3664627838</v>
       </c>
-      <c r="AB53" s="27" t="n">
+      <c r="AB53" s="23" t="n">
         <v>3595959571</v>
       </c>
       <c r="AC53" s="7" t="n">
@@ -12004,7 +11963,7 @@
         <v>1</v>
       </c>
       <c r="B60" s="16"/>
-      <c r="C60" s="28" t="s">
+      <c r="C60" s="24" t="s">
         <v>603</v>
       </c>
       <c r="D60" s="3" t="n">
@@ -12254,7 +12213,7 @@
       <c r="AA62" s="11" t="n">
         <v>904391025</v>
       </c>
-      <c r="AB62" s="29" t="n">
+      <c r="AB62" s="25" t="n">
         <v>901419307</v>
       </c>
       <c r="AC62" s="14" t="n">
@@ -12447,7 +12406,7 @@
       <c r="E65" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F65" s="30" t="n">
+      <c r="F65" s="26" t="n">
         <v>139442670</v>
       </c>
       <c r="G65" s="9" t="s">
@@ -12471,28 +12430,28 @@
       <c r="M65" s="9" t="s">
         <v>658</v>
       </c>
-      <c r="N65" s="30" t="n">
+      <c r="N65" s="26" t="n">
         <v>48977640</v>
       </c>
-      <c r="O65" s="31" t="s">
+      <c r="O65" s="27" t="s">
         <v>659</v>
       </c>
       <c r="P65" s="11" t="n">
         <v>45400500</v>
       </c>
-      <c r="Q65" s="31" t="s">
+      <c r="Q65" s="27" t="s">
         <v>660</v>
       </c>
       <c r="R65" s="11" t="n">
         <v>44450000</v>
       </c>
-      <c r="S65" s="31" t="s">
+      <c r="S65" s="27" t="s">
         <v>661</v>
       </c>
       <c r="T65" s="11" t="n">
         <v>35652810</v>
       </c>
-      <c r="U65" s="31" t="s">
+      <c r="U65" s="27" t="s">
         <v>662</v>
       </c>
       <c r="V65" s="11" t="n">
@@ -12514,7 +12473,7 @@
       <c r="AA65" s="11" t="n">
         <v>3621429969</v>
       </c>
-      <c r="AB65" s="32" t="n">
+      <c r="AB65" s="28" t="n">
         <v>3535402755</v>
       </c>
       <c r="AC65" s="14" t="n">
@@ -12881,7 +12840,7 @@
       <c r="E70" s="9" t="s">
         <v>703</v>
       </c>
-      <c r="F70" s="33" t="n">
+      <c r="F70" s="29" t="n">
         <v>109936552</v>
       </c>
       <c r="G70" s="9" t="s">
@@ -12941,7 +12900,7 @@
       <c r="Z70" s="13" t="n">
         <v>2014</v>
       </c>
-      <c r="AA70" s="34" t="n">
+      <c r="AA70" s="30" t="n">
         <v>1527677336</v>
       </c>
       <c r="AB70" s="11" t="n">
@@ -13384,7 +13343,7 @@
       <c r="AA75" s="5" t="n">
         <v>1036999800</v>
       </c>
-      <c r="AB75" s="27" t="n">
+      <c r="AB75" s="23" t="n">
         <v>1033225640</v>
       </c>
       <c r="AC75" s="7" t="n">
@@ -17402,7 +17361,7 @@
       <c r="AB122" s="5" t="n">
         <v>366624276</v>
       </c>
-      <c r="AC122" s="35" t="n">
+      <c r="AC122" s="31" t="n">
         <v>42849</v>
       </c>
     </row>
@@ -17943,16 +17902,16 @@
       <c r="D129" s="10" t="n">
         <v>2013</v>
       </c>
-      <c r="E129" s="36" t="s">
+      <c r="E129" s="32" t="s">
         <v>1244</v>
       </c>
-      <c r="F129" s="37" t="n">
+      <c r="F129" s="33" t="n">
         <v>42567580</v>
       </c>
       <c r="G129" s="12" t="s">
         <v>1245</v>
       </c>
-      <c r="H129" s="37" t="n">
+      <c r="H129" s="33" t="n">
         <v>23450000</v>
       </c>
       <c r="I129" s="12" t="s">
@@ -17982,25 +17941,25 @@
       <c r="Q129" s="12" t="s">
         <v>1249</v>
       </c>
-      <c r="R129" s="37" t="n">
+      <c r="R129" s="33" t="n">
         <v>8864800</v>
       </c>
       <c r="S129" s="12" t="s">
         <v>1250</v>
       </c>
-      <c r="T129" s="37" t="n">
+      <c r="T129" s="33" t="n">
         <v>8482450</v>
       </c>
       <c r="U129" s="12" t="s">
         <v>1251</v>
       </c>
-      <c r="V129" s="37" t="n">
+      <c r="V129" s="33" t="n">
         <v>8464400</v>
       </c>
       <c r="W129" s="12" t="s">
         <v>1252</v>
       </c>
-      <c r="X129" s="37" t="n">
+      <c r="X129" s="33" t="n">
         <v>6478380</v>
       </c>
       <c r="Y129" s="11" t="n">
@@ -18366,7 +18325,7 @@
       <c r="AB133" s="11" t="n">
         <v>3828716963</v>
       </c>
-      <c r="AC133" s="38" t="n">
+      <c r="AC133" s="34" t="n">
         <v>41934</v>
       </c>
     </row>
@@ -18715,7 +18674,7 @@
       <c r="F138" s="5" t="n">
         <v>35466894</v>
       </c>
-      <c r="G138" s="39" t="s">
+      <c r="G138" s="35" t="s">
         <v>1328</v>
       </c>
       <c r="H138" s="5" t="n">
@@ -21004,7 +20963,7 @@
       <c r="E165" s="9" t="s">
         <v>1574</v>
       </c>
-      <c r="F165" s="33" t="n">
+      <c r="F165" s="29" t="n">
         <v>75569410</v>
       </c>
       <c r="G165" s="9" t="s">
@@ -21016,7 +20975,7 @@
       <c r="I165" s="9" t="s">
         <v>1576</v>
       </c>
-      <c r="J165" s="40" t="n">
+      <c r="J165" s="36" t="n">
         <v>58051391</v>
       </c>
       <c r="K165" s="9" t="s">
@@ -21168,7 +21127,7 @@
       <c r="C167" s="8" t="s">
         <v>1594</v>
       </c>
-      <c r="D167" s="41" t="n">
+      <c r="D167" s="37" t="n">
         <v>2015</v>
       </c>
       <c r="E167" s="8" t="s">
@@ -21177,13 +21136,13 @@
       <c r="F167" s="8" t="n">
         <v>10935550</v>
       </c>
-      <c r="G167" s="42" t="s">
+      <c r="G167" s="22" t="s">
         <v>1520</v>
       </c>
-      <c r="H167" s="42" t="n">
+      <c r="H167" s="22" t="n">
         <v>4516510</v>
       </c>
-      <c r="I167" s="43" t="s">
+      <c r="I167" s="38" t="s">
         <v>1595</v>
       </c>
       <c r="J167" s="8" t="n">
@@ -21231,11 +21190,11 @@
       <c r="X167" s="8" t="n">
         <v>2058120</v>
       </c>
-      <c r="Y167" s="43" t="n">
+      <c r="Y167" s="38" t="n">
         <f aca="false">SUM(F167:X167)</f>
         <v>36286064</v>
       </c>
-      <c r="Z167" s="43" t="n">
+      <c r="Z167" s="38" t="n">
         <v>2015</v>
       </c>
       <c r="AA167" s="8" t="n">
@@ -21244,7 +21203,7 @@
       <c r="AB167" s="8" t="n">
         <v>1279189398</v>
       </c>
-      <c r="AC167" s="44" t="n">
+      <c r="AC167" s="39" t="n">
         <v>42871</v>
       </c>
     </row>
@@ -21570,7 +21529,7 @@
       <c r="X172" s="11"/>
       <c r="Y172" s="11"/>
       <c r="Z172" s="13"/>
-      <c r="AA172" s="45"/>
+      <c r="AA172" s="40"/>
       <c r="AB172" s="11"/>
       <c r="AC172" s="14"/>
     </row>
@@ -22672,45 +22631,46 @@
   <dimension ref="A1:IW174"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="X151" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D118" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="X1" activeCellId="0" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="A151" activeCellId="0" sqref="A151"/>
-      <selection pane="bottomRight" activeCell="AE176" activeCellId="0" sqref="AE176"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A118" activeCellId="0" sqref="A118"/>
+      <selection pane="bottomRight" activeCell="G142" activeCellId="0" sqref="G142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="61.015306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="9" width="46.1683673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="11" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="11" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="9" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="11" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="9" width="43.7397959183673"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="11" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="9" width="38.3367346938776"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="11" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="9" width="49.4081632653061"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="11" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="9" width="65.6071428571429"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="11" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="9" width="40.765306122449"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="11" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="9" width="39.5510204081633"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="11" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="11" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="13" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="11" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="11" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="14" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="257" min="30" style="9" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="59.530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="9" width="44.9540816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="11" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="11" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="9" width="41.7142857142857"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="11" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="9" width="42.6581632653061"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="11" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="9" width="37.3928571428571"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="11" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="9" width="48.3265306122449"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="11" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="9" width="64.1224489795918"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="11" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="9" width="39.8214285714286"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="11" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="9" width="38.6071428571429"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="11" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="11" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="13" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="11" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="11" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="14" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="257" min="30" style="9" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26630,31 +26590,31 @@
       <c r="D46" s="3" t="n">
         <v>2014</v>
       </c>
-      <c r="E46" s="46" t="s">
+      <c r="E46" s="41" t="s">
         <v>469</v>
       </c>
       <c r="F46" s="5" t="n">
         <v>22238610</v>
       </c>
-      <c r="G46" s="47" t="s">
+      <c r="G46" s="19" t="s">
         <v>470</v>
       </c>
       <c r="H46" s="5" t="n">
         <v>21993860</v>
       </c>
-      <c r="I46" s="47" t="s">
+      <c r="I46" s="19" t="s">
         <v>471</v>
       </c>
       <c r="J46" s="5" t="n">
         <v>19242110</v>
       </c>
-      <c r="K46" s="47" t="s">
+      <c r="K46" s="19" t="s">
         <v>472</v>
       </c>
-      <c r="L46" s="48" t="n">
+      <c r="L46" s="20" t="n">
         <v>15487800</v>
       </c>
-      <c r="M46" s="47" t="s">
+      <c r="M46" s="19" t="s">
         <v>101</v>
       </c>
       <c r="N46" s="5" t="n">
@@ -26666,28 +26626,28 @@
       <c r="P46" s="5" t="n">
         <v>10859990</v>
       </c>
-      <c r="Q46" s="47" t="s">
+      <c r="Q46" s="19" t="s">
         <v>1777</v>
       </c>
       <c r="R46" s="5" t="n">
         <v>9840590</v>
       </c>
-      <c r="S46" s="46" t="s">
+      <c r="S46" s="41" t="s">
         <v>1778</v>
       </c>
       <c r="T46" s="5" t="n">
         <v>8776440</v>
       </c>
-      <c r="U46" s="47" t="s">
+      <c r="U46" s="19" t="s">
         <v>294</v>
       </c>
       <c r="V46" s="5" t="n">
         <v>8370880</v>
       </c>
-      <c r="W46" s="47" t="s">
+      <c r="W46" s="19" t="s">
         <v>1779</v>
       </c>
-      <c r="X46" s="48" t="n">
+      <c r="X46" s="20" t="n">
         <v>8184460</v>
       </c>
       <c r="Y46" s="5" t="n">
@@ -27050,7 +27010,7 @@
         <v>42159</v>
       </c>
     </row>
-    <row r="51" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="n">
         <v>1</v>
       </c>
@@ -27138,7 +27098,7 @@
         <v>42146</v>
       </c>
     </row>
-    <row r="52" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="n">
         <v>1</v>
       </c>
@@ -27307,7 +27267,7 @@
       <c r="AA53" s="5" t="n">
         <v>3594688850</v>
       </c>
-      <c r="AB53" s="27" t="n">
+      <c r="AB53" s="23" t="n">
         <v>3533281325</v>
       </c>
       <c r="AC53" s="7" t="n">
@@ -27824,7 +27784,7 @@
         <v>1</v>
       </c>
       <c r="B60" s="16"/>
-      <c r="C60" s="28" t="s">
+      <c r="C60" s="24" t="s">
         <v>603</v>
       </c>
       <c r="D60" s="3" t="n">
@@ -28070,7 +28030,7 @@
       <c r="AA62" s="11" t="n">
         <v>904391025</v>
       </c>
-      <c r="AB62" s="29" t="n">
+      <c r="AB62" s="25" t="n">
         <v>901419307</v>
       </c>
       <c r="AC62" s="14" t="n">
@@ -28264,7 +28224,7 @@
       <c r="E65" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F65" s="30" t="n">
+      <c r="F65" s="26" t="n">
         <v>139442670</v>
       </c>
       <c r="G65" s="9" t="s">
@@ -28288,28 +28248,28 @@
       <c r="M65" s="9" t="s">
         <v>658</v>
       </c>
-      <c r="N65" s="30" t="n">
+      <c r="N65" s="26" t="n">
         <v>48977640</v>
       </c>
-      <c r="O65" s="31" t="s">
+      <c r="O65" s="27" t="s">
         <v>659</v>
       </c>
       <c r="P65" s="11" t="n">
         <v>45400500</v>
       </c>
-      <c r="Q65" s="31" t="s">
+      <c r="Q65" s="27" t="s">
         <v>660</v>
       </c>
       <c r="R65" s="11" t="n">
         <v>44450000</v>
       </c>
-      <c r="S65" s="31" t="s">
+      <c r="S65" s="27" t="s">
         <v>661</v>
       </c>
       <c r="T65" s="11" t="n">
         <v>35652810</v>
       </c>
-      <c r="U65" s="31" t="s">
+      <c r="U65" s="27" t="s">
         <v>662</v>
       </c>
       <c r="V65" s="11" t="n">
@@ -28331,7 +28291,7 @@
       <c r="AA65" s="11" t="n">
         <v>3621429969</v>
       </c>
-      <c r="AB65" s="32" t="n">
+      <c r="AB65" s="28" t="n">
         <v>3535402755</v>
       </c>
       <c r="AC65" s="14" t="n">
@@ -28703,7 +28663,7 @@
       <c r="E70" s="2" t="s">
         <v>703</v>
       </c>
-      <c r="F70" s="49" t="n">
+      <c r="F70" s="42" t="n">
         <v>109936552</v>
       </c>
       <c r="G70" s="2" t="s">
@@ -28762,7 +28722,7 @@
       <c r="Z70" s="6" t="n">
         <v>2014</v>
       </c>
-      <c r="AA70" s="50" t="n">
+      <c r="AA70" s="43" t="n">
         <v>1527677336</v>
       </c>
       <c r="AB70" s="5" t="n">
@@ -29172,7 +29132,7 @@
       <c r="AA75" s="11" t="n">
         <v>1034480809</v>
       </c>
-      <c r="AB75" s="40" t="n">
+      <c r="AB75" s="36" t="n">
         <v>1030897219</v>
       </c>
       <c r="AC75" s="14" t="n">
@@ -33067,7 +33027,7 @@
       <c r="AB122" s="5" t="n">
         <v>366726656</v>
       </c>
-      <c r="AC122" s="35" t="n">
+      <c r="AC122" s="31" t="n">
         <v>42166</v>
       </c>
     </row>
@@ -33601,16 +33561,16 @@
       <c r="D129" s="10" t="n">
         <v>2013</v>
       </c>
-      <c r="E129" s="36" t="s">
+      <c r="E129" s="32" t="s">
         <v>1244</v>
       </c>
-      <c r="F129" s="37" t="n">
+      <c r="F129" s="33" t="n">
         <v>42567580</v>
       </c>
       <c r="G129" s="12" t="s">
         <v>1245</v>
       </c>
-      <c r="H129" s="37" t="n">
+      <c r="H129" s="33" t="n">
         <v>23450000</v>
       </c>
       <c r="I129" s="12" t="s">
@@ -33640,25 +33600,25 @@
       <c r="Q129" s="12" t="s">
         <v>1249</v>
       </c>
-      <c r="R129" s="37" t="n">
+      <c r="R129" s="33" t="n">
         <v>8864800</v>
       </c>
       <c r="S129" s="12" t="s">
         <v>1250</v>
       </c>
-      <c r="T129" s="37" t="n">
+      <c r="T129" s="33" t="n">
         <v>8482450</v>
       </c>
       <c r="U129" s="12" t="s">
         <v>1251</v>
       </c>
-      <c r="V129" s="37" t="n">
+      <c r="V129" s="33" t="n">
         <v>8464400</v>
       </c>
       <c r="W129" s="12" t="s">
         <v>1252</v>
       </c>
-      <c r="X129" s="37" t="n">
+      <c r="X129" s="33" t="n">
         <v>6478380</v>
       </c>
       <c r="Y129" s="11" t="n">
@@ -34026,7 +33986,7 @@
       <c r="AB133" s="5" t="n">
         <v>3828716963</v>
       </c>
-      <c r="AC133" s="51" t="n">
+      <c r="AC133" s="44" t="n">
         <v>41934</v>
       </c>
     </row>
@@ -34393,7 +34353,7 @@
       <c r="F138" s="5" t="n">
         <v>31034387</v>
       </c>
-      <c r="G138" s="39" t="s">
+      <c r="G138" s="35" t="s">
         <v>2054</v>
       </c>
       <c r="H138" s="5" t="n">
@@ -36657,7 +36617,7 @@
       <c r="E165" s="2" t="s">
         <v>1574</v>
       </c>
-      <c r="F165" s="49" t="n">
+      <c r="F165" s="42" t="n">
         <v>74746247</v>
       </c>
       <c r="G165" s="2" t="s">
@@ -36669,7 +36629,7 @@
       <c r="I165" s="2" t="s">
         <v>1577</v>
       </c>
-      <c r="J165" s="27" t="n">
+      <c r="J165" s="23" t="n">
         <v>60367098</v>
       </c>
       <c r="K165" s="2" t="s">
@@ -36819,7 +36779,7 @@
       <c r="C167" s="1" t="s">
         <v>1594</v>
       </c>
-      <c r="D167" s="52" t="n">
+      <c r="D167" s="45" t="n">
         <v>2014</v>
       </c>
       <c r="E167" s="1" t="s">
@@ -36828,7 +36788,7 @@
       <c r="F167" s="0" t="n">
         <v>10396340</v>
       </c>
-      <c r="G167" s="53" t="s">
+      <c r="G167" s="46" t="s">
         <v>1520</v>
       </c>
       <c r="H167" s="0" t="n">
@@ -36895,7 +36855,7 @@
       <c r="AB167" s="1" t="n">
         <v>1268176081</v>
       </c>
-      <c r="AC167" s="54" t="n">
+      <c r="AC167" s="47" t="n">
         <v>42140</v>
       </c>
       <c r="AD167" s="1"/>
@@ -37395,7 +37355,7 @@
       <c r="B171" s="16"/>
     </row>
     <row r="172" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA172" s="45"/>
+      <c r="AA172" s="40"/>
     </row>
     <row r="174" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="9" t="n">

</xml_diff>